<commit_message>
delete teaching materials and change the corresponding description
</commit_message>
<xml_diff>
--- a/仓库资源/资源信息表.xlsx
+++ b/仓库资源/资源信息表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uestc-course\仓库资源\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9215B605-C22C-4796-BCD1-C237F743DAA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BB325-F5D8-41C4-A4AB-4A07026B93BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{C3119D50-7D9A-4B03-9531-E4F1E5BC8828}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>复习资料</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,27 +95,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文件夹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>授课老师</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文件个数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>考试类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>考试时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>课件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -298,16 +282,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3FE90A-5041-44C9-97AF-19E7F071E39C}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -636,16 +620,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -678,10 +662,10 @@
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -690,8 +674,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
@@ -700,8 +684,8 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -710,8 +694,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -720,8 +704,8 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -730,8 +714,8 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -756,10 +740,10 @@
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -850,11 +834,11 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
@@ -862,9 +846,9 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
@@ -872,9 +856,9 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -882,9 +866,9 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
@@ -892,9 +876,9 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -902,9 +886,9 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -934,11 +918,11 @@
       <c r="E24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
@@ -946,9 +930,9 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
@@ -956,9 +940,9 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
@@ -966,9 +950,9 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -976,9 +960,9 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
@@ -986,13 +970,13 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1002,23 +986,25 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
@@ -1072,106 +1058,12 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
+  <mergeCells count="24">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A30:H30"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="F17:H17"/>
@@ -1183,6 +1075,15 @@
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="7">
@@ -1200,7 +1101,7 @@
       <formula1>"期末考试,期中考试,课堂考试,补考,重修"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文件名" prompt="[作业时间]-[作业类型]，示例如下：_x000a__x000a_2019年春-课后作业_x000a_2018年秋-课堂作业-1_x000a_2018年秋-课堂作业-2" sqref="B25:B29" xr:uid="{94147929-C548-48AC-B5A9-2FEC763FB6C0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文件夹命名" prompt="[课程名]-[课件制作人]，示例：_x000a__x000a_中国特色社会主义理论与实践研究-制作人1_x000a_中国特色社会主义理论与实践研究-制作人2" sqref="B32:B36 B39:B43" xr:uid="{3E447807-70D2-4D74-B70B-EC942E1AA13C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文件夹命名" prompt="[课程名]-[课件制作人]，示例：_x000a__x000a_中国特色社会主义理论与实践研究-制作人1_x000a_中国特色社会主义理论与实践研究-制作人2" sqref="B32:B36" xr:uid="{3E447807-70D2-4D74-B70B-EC942E1AA13C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Delete teaching materials (#11)
删除了仓库内课件相关内容。

此决定基于以下几方面考量：

 - 版权
 - 课件并不是学生复习难以获取的资料

故仓库暂时不考虑收录课件。
</commit_message>
<xml_diff>
--- a/仓库资源/资源信息表.xlsx
+++ b/仓库资源/资源信息表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uestc-course\仓库资源\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9215B605-C22C-4796-BCD1-C237F743DAA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BB325-F5D8-41C4-A4AB-4A07026B93BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{C3119D50-7D9A-4B03-9531-E4F1E5BC8828}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>复习资料</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,27 +95,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文件夹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>授课老师</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文件个数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>考试类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>考试时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>课件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -298,16 +282,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3FE90A-5041-44C9-97AF-19E7F071E39C}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -636,16 +620,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -678,10 +662,10 @@
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -690,8 +674,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
@@ -700,8 +684,8 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -710,8 +694,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -720,8 +704,8 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -730,8 +714,8 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -756,10 +740,10 @@
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -850,11 +834,11 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
@@ -862,9 +846,9 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
@@ -872,9 +856,9 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
@@ -882,9 +866,9 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
@@ -892,9 +876,9 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -902,9 +886,9 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -934,11 +918,11 @@
       <c r="E24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
@@ -946,9 +930,9 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
@@ -956,9 +940,9 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
@@ -966,9 +950,9 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -976,9 +960,9 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
@@ -986,13 +970,13 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1002,23 +986,25 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
@@ -1072,106 +1058,12 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
+  <mergeCells count="24">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A30:H30"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="F17:H17"/>
@@ -1183,6 +1075,15 @@
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="7">
@@ -1200,7 +1101,7 @@
       <formula1>"期末考试,期中考试,课堂考试,补考,重修"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文件名" prompt="[作业时间]-[作业类型]，示例如下：_x000a__x000a_2019年春-课后作业_x000a_2018年秋-课堂作业-1_x000a_2018年秋-课堂作业-2" sqref="B25:B29" xr:uid="{94147929-C548-48AC-B5A9-2FEC763FB6C0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文件夹命名" prompt="[课程名]-[课件制作人]，示例：_x000a__x000a_中国特色社会主义理论与实践研究-制作人1_x000a_中国特色社会主义理论与实践研究-制作人2" sqref="B32:B36 B39:B43" xr:uid="{3E447807-70D2-4D74-B70B-EC942E1AA13C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="文件夹命名" prompt="[课程名]-[课件制作人]，示例：_x000a__x000a_中国特色社会主义理论与实践研究-制作人1_x000a_中国特色社会主义理论与实践研究-制作人2" sqref="B32:B36" xr:uid="{3E447807-70D2-4D74-B70B-EC942E1AA13C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>